<commit_message>
Added more levels and made the level parser work
</commit_message>
<xml_diff>
--- a/assets/levels/Level Maker.xlsx
+++ b/assets/levels/Level Maker.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyad Abdelazim\Documents\Learning\LoC\sokoban\levels\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyad Abdelazim\Documents\Learning\LoC\sokoban\assets\levels\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D8AA1A4-279A-4EC4-8331-BCC0D04337D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A785CD51-9E27-4C9B-9143-448FE6A5B688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{06C2B5DF-9460-49A2-A75E-D26C26CFECCD}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="7">
   <si>
     <t>#</t>
   </si>
@@ -500,10 +500,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CF64F46-213D-4C9A-B903-0755EAA6CD50}">
-  <dimension ref="A1:AL41"/>
+  <dimension ref="A1:AL85"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="AJ33" sqref="AJ33"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="0">
+      <selection activeCell="A65" sqref="A65:AD85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4311,6 +4311,3348 @@
         <v>+</v>
       </c>
     </row>
+    <row r="42" spans="1:31" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="43" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2"/>
+      <c r="I43" s="2"/>
+      <c r="J43" s="2"/>
+      <c r="K43" s="2"/>
+      <c r="L43" s="2"/>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="2"/>
+      <c r="Q43" s="2"/>
+      <c r="R43" s="2"/>
+      <c r="S43" s="2"/>
+      <c r="T43" s="2"/>
+      <c r="U43" s="2"/>
+      <c r="V43" s="2"/>
+      <c r="W43" s="2"/>
+      <c r="X43" s="2"/>
+      <c r="Y43" s="2"/>
+      <c r="Z43" s="2"/>
+      <c r="AA43" s="2"/>
+      <c r="AB43" s="2"/>
+      <c r="AC43" s="2"/>
+      <c r="AD43" s="3"/>
+    </row>
+    <row r="44" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A44" s="4"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
+      <c r="H44" s="5"/>
+      <c r="I44" s="5"/>
+      <c r="J44" s="5"/>
+      <c r="K44" s="5"/>
+      <c r="L44" s="5"/>
+      <c r="M44" s="5"/>
+      <c r="N44" s="5"/>
+      <c r="O44" s="5"/>
+      <c r="P44" s="5"/>
+      <c r="Q44" s="5"/>
+      <c r="R44" s="5"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="5"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="5"/>
+      <c r="W44" s="5"/>
+      <c r="X44" s="5"/>
+      <c r="Y44" s="5"/>
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="5"/>
+      <c r="AC44" s="5"/>
+      <c r="AD44" s="6"/>
+    </row>
+    <row r="45" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A45" s="4"/>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
+      <c r="L45" s="5"/>
+      <c r="M45" s="5"/>
+      <c r="N45" s="5"/>
+      <c r="O45" s="5"/>
+      <c r="P45" s="5"/>
+      <c r="Q45" s="5"/>
+      <c r="R45" s="5"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="5"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="5"/>
+      <c r="W45" s="5"/>
+      <c r="X45" s="5"/>
+      <c r="Y45" s="5"/>
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="5"/>
+      <c r="AC45" s="5"/>
+      <c r="AD45" s="6"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="5"/>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="11"/>
+      <c r="F46" s="11"/>
+      <c r="G46" s="11"/>
+      <c r="H46" s="11"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
+      <c r="L46" s="5"/>
+      <c r="M46" s="5"/>
+      <c r="N46" s="5"/>
+      <c r="O46" s="5"/>
+      <c r="P46" s="5"/>
+      <c r="Q46" s="5"/>
+      <c r="R46" s="5"/>
+      <c r="S46" s="5"/>
+      <c r="T46" s="5"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="5"/>
+      <c r="W46" s="5"/>
+      <c r="X46" s="5"/>
+      <c r="Y46" s="5"/>
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="5"/>
+      <c r="AC46" s="5"/>
+      <c r="AD46" s="6"/>
+    </row>
+    <row r="47" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A47" s="4"/>
+      <c r="B47" s="5"/>
+      <c r="C47" s="5"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
+      <c r="H47" s="11"/>
+      <c r="I47" s="5"/>
+      <c r="J47" s="5"/>
+      <c r="K47" s="5"/>
+      <c r="L47" s="10"/>
+      <c r="M47" s="10"/>
+      <c r="N47" s="10"/>
+      <c r="O47" s="10"/>
+      <c r="P47" s="10"/>
+      <c r="Q47" s="10"/>
+      <c r="R47" s="10"/>
+      <c r="S47" s="10"/>
+      <c r="T47" s="10"/>
+      <c r="U47" s="10"/>
+      <c r="V47" s="10"/>
+      <c r="W47" s="10"/>
+      <c r="X47" s="10"/>
+      <c r="Y47" s="5"/>
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="5"/>
+      <c r="AC47" s="5"/>
+      <c r="AD47" s="6"/>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A48" s="4"/>
+      <c r="B48" s="5"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="10"/>
+      <c r="G48" s="5"/>
+      <c r="H48" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="I48" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="5"/>
+      <c r="R48" s="5"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="5"/>
+      <c r="U48" s="5"/>
+      <c r="V48" s="5"/>
+      <c r="W48" s="5"/>
+      <c r="X48" s="5"/>
+      <c r="Y48" s="5"/>
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="5"/>
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="6"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A49" s="4"/>
+      <c r="B49" s="5"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
+      <c r="H49" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I49" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="J49" s="11"/>
+      <c r="K49" s="11"/>
+      <c r="L49" s="10"/>
+      <c r="M49" s="10"/>
+      <c r="N49" s="10"/>
+      <c r="O49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="P49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="R49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="S49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="T49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="U49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="V49" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W49" s="5"/>
+      <c r="X49" s="5"/>
+      <c r="Y49" s="5"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="5"/>
+      <c r="AC49" s="5"/>
+      <c r="AD49" s="6"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A50" s="4"/>
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="10"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="I50" s="10"/>
+      <c r="J50" s="10"/>
+      <c r="K50" s="11"/>
+      <c r="L50" s="10"/>
+      <c r="M50" s="10"/>
+      <c r="N50" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O50" s="10"/>
+      <c r="P50" s="5"/>
+      <c r="Q50" s="5"/>
+      <c r="R50" s="5"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="5"/>
+      <c r="U50" s="5"/>
+      <c r="V50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="W50" s="5"/>
+      <c r="X50" s="5"/>
+      <c r="Y50" s="5"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="5"/>
+      <c r="AC50" s="5"/>
+      <c r="AD50" s="6"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A51" s="4"/>
+      <c r="B51" s="5"/>
+      <c r="C51" s="10"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="10"/>
+      <c r="H51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I51" s="5"/>
+      <c r="J51" s="10"/>
+      <c r="K51" s="11"/>
+      <c r="L51" s="5"/>
+      <c r="M51" s="5"/>
+      <c r="N51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="O51" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="P51" s="5"/>
+      <c r="Q51" s="10"/>
+      <c r="R51" s="10"/>
+      <c r="S51" s="10"/>
+      <c r="T51" s="10"/>
+      <c r="U51" s="10"/>
+      <c r="V51" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W51" s="5"/>
+      <c r="X51" s="5"/>
+      <c r="Y51" s="5"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="5"/>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="6"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A52" s="4"/>
+      <c r="B52" s="5"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="5"/>
+      <c r="E52" s="5"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="5"/>
+      <c r="H52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="11"/>
+      <c r="L52" s="11"/>
+      <c r="M52" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="N52" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="5"/>
+      <c r="S52" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="T52" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U52" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V52" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W52" s="10"/>
+      <c r="X52" s="5"/>
+      <c r="Y52" s="5"/>
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="5"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="6"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A53" s="4"/>
+      <c r="B53" s="5"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="5"/>
+      <c r="E53" s="5"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="I53" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J53" s="5"/>
+      <c r="K53" s="11"/>
+      <c r="L53" s="11"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O53" s="11"/>
+      <c r="P53" s="11"/>
+      <c r="Q53" s="11"/>
+      <c r="R53" s="11"/>
+      <c r="S53" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="T53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="U53" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V53" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W53" s="10"/>
+      <c r="X53" s="5"/>
+      <c r="Y53" s="5"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="5"/>
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="6"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A54" s="4"/>
+      <c r="B54" s="5"/>
+      <c r="C54" s="10"/>
+      <c r="D54" s="5"/>
+      <c r="E54" s="5"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="5"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="J54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="K54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="M54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="N54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="O54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="P54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="R54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="S54" s="11" t="s">
+        <v>0</v>
+      </c>
+      <c r="T54" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="U54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="V54" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="W54" s="5"/>
+      <c r="X54" s="5"/>
+      <c r="Y54" s="5"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="5"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="6"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A55" s="4"/>
+      <c r="B55" s="5"/>
+      <c r="C55" s="10"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5"/>
+      <c r="F55" s="10"/>
+      <c r="G55" s="10"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="10"/>
+      <c r="J55" s="10"/>
+      <c r="K55" s="11"/>
+      <c r="L55" s="11"/>
+      <c r="M55" s="10"/>
+      <c r="N55" s="10"/>
+      <c r="O55" s="5"/>
+      <c r="P55" s="10"/>
+      <c r="Q55" s="10"/>
+      <c r="R55" s="10"/>
+      <c r="S55" s="11"/>
+      <c r="T55" s="5"/>
+      <c r="U55" s="10"/>
+      <c r="V55" s="10"/>
+      <c r="W55" s="10"/>
+      <c r="X55" s="5"/>
+      <c r="Y55" s="5"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="5"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="6"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="5"/>
+      <c r="C56" s="5"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5"/>
+      <c r="F56" s="10"/>
+      <c r="G56" s="10"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="10"/>
+      <c r="J56" s="10"/>
+      <c r="K56" s="11"/>
+      <c r="L56" s="11"/>
+      <c r="M56" s="11"/>
+      <c r="N56" s="11"/>
+      <c r="O56" s="11"/>
+      <c r="P56" s="11"/>
+      <c r="Q56" s="10"/>
+      <c r="R56" s="10"/>
+      <c r="S56" s="11"/>
+      <c r="T56" s="5"/>
+      <c r="U56" s="10"/>
+      <c r="V56" s="5"/>
+      <c r="W56" s="10"/>
+      <c r="X56" s="5"/>
+      <c r="Y56" s="5"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="5"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="6"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A57" s="4"/>
+      <c r="B57" s="5"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="5"/>
+      <c r="E57" s="5"/>
+      <c r="F57" s="10"/>
+      <c r="G57" s="5"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="10"/>
+      <c r="J57" s="10"/>
+      <c r="K57" s="11"/>
+      <c r="L57" s="11"/>
+      <c r="M57" s="10"/>
+      <c r="N57" s="10"/>
+      <c r="O57" s="5"/>
+      <c r="P57" s="11"/>
+      <c r="Q57" s="11"/>
+      <c r="R57" s="11"/>
+      <c r="S57" s="11"/>
+      <c r="T57" s="5"/>
+      <c r="U57" s="10"/>
+      <c r="V57" s="10"/>
+      <c r="W57" s="5"/>
+      <c r="X57" s="5"/>
+      <c r="Y57" s="5"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="5"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="6"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A58" s="4"/>
+      <c r="B58" s="5"/>
+      <c r="C58" s="5"/>
+      <c r="D58" s="5"/>
+      <c r="E58" s="5"/>
+      <c r="F58" s="5"/>
+      <c r="G58" s="5"/>
+      <c r="H58" s="10"/>
+      <c r="I58" s="10"/>
+      <c r="J58" s="10"/>
+      <c r="K58" s="11"/>
+      <c r="L58" s="11"/>
+      <c r="M58" s="11"/>
+      <c r="N58" s="11"/>
+      <c r="O58" s="11"/>
+      <c r="P58" s="11"/>
+      <c r="Q58" s="5"/>
+      <c r="R58" s="10"/>
+      <c r="S58" s="10"/>
+      <c r="T58" s="5"/>
+      <c r="U58" s="5"/>
+      <c r="V58" s="5"/>
+      <c r="W58" s="5"/>
+      <c r="X58" s="5"/>
+      <c r="Y58" s="5"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="5"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="6"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A59" s="4"/>
+      <c r="B59" s="5"/>
+      <c r="C59" s="5"/>
+      <c r="D59" s="5"/>
+      <c r="E59" s="10"/>
+      <c r="F59" s="10"/>
+      <c r="G59" s="10"/>
+      <c r="H59" s="5"/>
+      <c r="I59" s="5"/>
+      <c r="J59" s="5"/>
+      <c r="K59" s="5"/>
+      <c r="L59" s="5"/>
+      <c r="M59" s="11"/>
+      <c r="N59" s="11"/>
+      <c r="O59" s="11"/>
+      <c r="P59" s="11"/>
+      <c r="Q59" s="5"/>
+      <c r="R59" s="10"/>
+      <c r="S59" s="10"/>
+      <c r="T59" s="10"/>
+      <c r="U59" s="10"/>
+      <c r="V59" s="10"/>
+      <c r="W59" s="10"/>
+      <c r="X59" s="10"/>
+      <c r="Y59" s="5"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="5"/>
+      <c r="AB59" s="5"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="6"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A60" s="4"/>
+      <c r="B60" s="5"/>
+      <c r="C60" s="5"/>
+      <c r="D60" s="5"/>
+      <c r="E60" s="10"/>
+      <c r="F60" s="10"/>
+      <c r="G60" s="10"/>
+      <c r="H60" s="10"/>
+      <c r="I60" s="10"/>
+      <c r="J60" s="10"/>
+      <c r="K60" s="10"/>
+      <c r="L60" s="5"/>
+      <c r="M60" s="11"/>
+      <c r="N60" s="11"/>
+      <c r="O60" s="11"/>
+      <c r="P60" s="5"/>
+      <c r="Q60" s="5"/>
+      <c r="R60" s="10"/>
+      <c r="S60" s="10"/>
+      <c r="T60" s="10"/>
+      <c r="U60" s="10"/>
+      <c r="V60" s="10"/>
+      <c r="W60" s="10"/>
+      <c r="X60" s="10"/>
+      <c r="Y60" s="5"/>
+      <c r="Z60" s="5"/>
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="5"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="6"/>
+    </row>
+    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A61" s="4"/>
+      <c r="B61" s="5"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="5"/>
+      <c r="E61" s="5"/>
+      <c r="F61" s="5"/>
+      <c r="G61" s="5"/>
+      <c r="H61" s="5"/>
+      <c r="I61" s="5"/>
+      <c r="J61" s="5"/>
+      <c r="K61" s="5"/>
+      <c r="L61" s="5"/>
+      <c r="M61" s="5"/>
+      <c r="N61" s="5"/>
+      <c r="O61" s="5"/>
+      <c r="P61" s="5"/>
+      <c r="Q61" s="5"/>
+      <c r="R61" s="5"/>
+      <c r="S61" s="5"/>
+      <c r="T61" s="5"/>
+      <c r="U61" s="5"/>
+      <c r="V61" s="5"/>
+      <c r="W61" s="5"/>
+      <c r="X61" s="5"/>
+      <c r="Y61" s="5"/>
+      <c r="Z61" s="5"/>
+      <c r="AA61" s="5"/>
+      <c r="AB61" s="5"/>
+      <c r="AC61" s="5"/>
+      <c r="AD61" s="6"/>
+    </row>
+    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A62" s="4"/>
+      <c r="B62" s="5"/>
+      <c r="C62" s="5"/>
+      <c r="D62" s="5"/>
+      <c r="E62" s="5"/>
+      <c r="F62" s="5"/>
+      <c r="G62" s="5"/>
+      <c r="H62" s="5"/>
+      <c r="I62" s="5"/>
+      <c r="J62" s="5"/>
+      <c r="K62" s="5"/>
+      <c r="L62" s="5"/>
+      <c r="M62" s="5"/>
+      <c r="N62" s="5"/>
+      <c r="O62" s="5"/>
+      <c r="P62" s="5"/>
+      <c r="Q62" s="5"/>
+      <c r="R62" s="5"/>
+      <c r="S62" s="5"/>
+      <c r="T62" s="5"/>
+      <c r="U62" s="5"/>
+      <c r="V62" s="5"/>
+      <c r="W62" s="5"/>
+      <c r="X62" s="5"/>
+      <c r="Y62" s="5"/>
+      <c r="Z62" s="5"/>
+      <c r="AA62" s="5"/>
+      <c r="AB62" s="5"/>
+      <c r="AC62" s="5"/>
+      <c r="AD62" s="6"/>
+    </row>
+    <row r="63" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A63" s="7"/>
+      <c r="B63" s="8"/>
+      <c r="C63" s="8"/>
+      <c r="D63" s="8"/>
+      <c r="E63" s="8"/>
+      <c r="F63" s="8"/>
+      <c r="G63" s="8"/>
+      <c r="H63" s="8"/>
+      <c r="I63" s="8"/>
+      <c r="J63" s="8"/>
+      <c r="K63" s="8"/>
+      <c r="L63" s="8"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="8"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="8"/>
+      <c r="R63" s="8"/>
+      <c r="S63" s="8"/>
+      <c r="T63" s="8"/>
+      <c r="U63" s="8"/>
+      <c r="V63" s="8"/>
+      <c r="W63" s="8"/>
+      <c r="X63" s="8"/>
+      <c r="Y63" s="8"/>
+      <c r="Z63" s="8"/>
+      <c r="AA63" s="8"/>
+      <c r="AB63" s="8"/>
+      <c r="AC63" s="8"/>
+      <c r="AD63" s="9"/>
+    </row>
+    <row r="64" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="65" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A65" s="1" t="str">
+        <f>IF(OR(A44=" ", A44=""),"-",A44)</f>
+        <v>-</v>
+      </c>
+      <c r="B65" s="2" t="str">
+        <f t="shared" ref="B65:AD65" si="20">IF(OR(B44=" ", B44=""),"-",B44)</f>
+        <v>-</v>
+      </c>
+      <c r="C65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="D65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="E65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="F65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="G65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="H65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="I65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="J65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="K65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="L65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="M65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="N65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="O65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="P65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="Q65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="R65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="S65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="T65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="U65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="V65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="W65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="X65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="Y65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="Z65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="AA65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="AB65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="AC65" s="2" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+      <c r="AD65" s="3" t="str">
+        <f t="shared" si="20"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="66" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A66" s="4" t="str">
+        <f t="shared" ref="A66:AD66" si="21">IF(OR(A45=" ", A45=""),"-",A45)</f>
+        <v>-</v>
+      </c>
+      <c r="B66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="C66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="D66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="E66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="F66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="G66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="H66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="I66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="J66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="K66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="L66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="M66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="N66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="O66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="P66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="Q66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="R66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="S66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="T66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="U66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="V66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="W66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="X66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="Y66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="Z66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="AA66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="AB66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="AC66" s="5" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+      <c r="AD66" s="6" t="str">
+        <f t="shared" si="21"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A67" s="4" t="str">
+        <f t="shared" ref="A67:AD67" si="22">IF(OR(A46=" ", A46=""),"-",A46)</f>
+        <v>-</v>
+      </c>
+      <c r="B67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="C67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="D67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="E67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="F67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="G67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="H67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="I67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="J67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="K67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="L67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="M67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="N67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="O67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="P67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="Q67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="R67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="S67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="T67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="U67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="V67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="W67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="X67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="Y67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="Z67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="AA67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="AB67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="AC67" s="5" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+      <c r="AD67" s="6" t="str">
+        <f t="shared" si="22"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A68" s="4" t="str">
+        <f t="shared" ref="A68:AD68" si="23">IF(OR(A47=" ", A47=""),"-",A47)</f>
+        <v>-</v>
+      </c>
+      <c r="B68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="C68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="D68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="E68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="F68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="G68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="H68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="I68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="J68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="K68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="L68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="M68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="N68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="O68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="P68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="Q68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="R68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="S68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="T68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="U68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="V68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="W68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="X68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="Y68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="Z68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="AA68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="AB68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="AC68" s="5" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+      <c r="AD68" s="6" t="str">
+        <f t="shared" si="23"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A69" s="4" t="str">
+        <f t="shared" ref="A69:AD69" si="24">IF(OR(A48=" ", A48=""),"-",A48)</f>
+        <v>-</v>
+      </c>
+      <c r="B69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="C69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="D69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="E69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="F69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="G69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="H69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="I69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="J69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="K69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="L69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="M69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="N69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="O69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>#</v>
+      </c>
+      <c r="P69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="Q69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="R69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="S69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="T69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="U69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="V69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="W69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="X69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="Y69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="Z69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="AA69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="AB69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="AC69" s="5" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+      <c r="AD69" s="6" t="str">
+        <f t="shared" si="24"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A70" s="4" t="str">
+        <f t="shared" ref="A70:AD70" si="25">IF(OR(A49=" ", A49=""),"-",A49)</f>
+        <v>-</v>
+      </c>
+      <c r="B70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="C70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="D70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="E70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="F70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="G70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="H70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="I70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>@</v>
+      </c>
+      <c r="J70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="K70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="L70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="M70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="N70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="O70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="P70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="Q70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="R70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="S70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="T70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="U70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="V70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>#</v>
+      </c>
+      <c r="W70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="X70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="Y70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="Z70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="AA70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="AB70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="AC70" s="5" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+      <c r="AD70" s="6" t="str">
+        <f t="shared" si="25"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A71" s="4" t="str">
+        <f t="shared" ref="A71:AD71" si="26">IF(OR(A50=" ", A50=""),"-",A50)</f>
+        <v>-</v>
+      </c>
+      <c r="B71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="C71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="D71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="E71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="F71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="G71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="H71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>#</v>
+      </c>
+      <c r="I71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="J71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="K71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="L71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="M71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="N71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>$</v>
+      </c>
+      <c r="O71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="P71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="Q71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="R71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="S71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="T71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="U71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="V71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>#</v>
+      </c>
+      <c r="W71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="X71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="Y71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="Z71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="AA71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="AB71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="AC71" s="5" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+      <c r="AD71" s="6" t="str">
+        <f t="shared" si="26"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A72" s="4" t="str">
+        <f t="shared" ref="A72:AD72" si="27">IF(OR(A51=" ", A51=""),"-",A51)</f>
+        <v>-</v>
+      </c>
+      <c r="B72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="C72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="D72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="E72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="F72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="G72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="H72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>#</v>
+      </c>
+      <c r="I72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="J72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="K72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="L72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="M72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="N72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>$</v>
+      </c>
+      <c r="O72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>$</v>
+      </c>
+      <c r="P72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="Q72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="R72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="S72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="T72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="U72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="V72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>#</v>
+      </c>
+      <c r="W72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="X72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="Y72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="Z72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="AA72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="AB72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="AC72" s="5" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+      <c r="AD72" s="6" t="str">
+        <f t="shared" si="27"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A73" s="4" t="str">
+        <f t="shared" ref="A73:AD73" si="28">IF(OR(A52=" ", A52=""),"-",A52)</f>
+        <v>-</v>
+      </c>
+      <c r="B73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="C73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="D73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="E73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="F73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="G73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="H73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>#</v>
+      </c>
+      <c r="I73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="J73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="K73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="L73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="M73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>$</v>
+      </c>
+      <c r="N73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>$</v>
+      </c>
+      <c r="O73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="P73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="Q73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="R73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="S73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>.</v>
+      </c>
+      <c r="T73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>.</v>
+      </c>
+      <c r="U73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>.</v>
+      </c>
+      <c r="V73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>#</v>
+      </c>
+      <c r="W73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="X73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="Y73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="Z73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="AA73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="AB73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="AC73" s="5" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+      <c r="AD73" s="6" t="str">
+        <f t="shared" si="28"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A74" s="4" t="str">
+        <f t="shared" ref="A74:AD74" si="29">IF(OR(A53=" ", A53=""),"-",A53)</f>
+        <v>-</v>
+      </c>
+      <c r="B74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="C74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="D74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="E74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="F74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="G74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="H74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>#</v>
+      </c>
+      <c r="I74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>#</v>
+      </c>
+      <c r="J74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="K74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="L74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="M74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="N74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>$</v>
+      </c>
+      <c r="O74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="P74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="Q74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="R74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="S74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>.</v>
+      </c>
+      <c r="T74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>.</v>
+      </c>
+      <c r="U74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>.</v>
+      </c>
+      <c r="V74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>#</v>
+      </c>
+      <c r="W74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="X74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="Y74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="Z74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="AA74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="AB74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="AC74" s="5" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+      <c r="AD74" s="6" t="str">
+        <f t="shared" si="29"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="75" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A75" s="4" t="str">
+        <f t="shared" ref="A75:AD75" si="30">IF(OR(A54=" ", A54=""),"-",A54)</f>
+        <v>-</v>
+      </c>
+      <c r="B75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="C75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="D75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="E75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="F75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="G75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="H75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="I75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="J75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="K75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="L75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="M75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="N75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="O75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="P75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="Q75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="R75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="S75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="T75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="U75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="V75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>#</v>
+      </c>
+      <c r="W75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="X75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="Y75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="Z75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="AA75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="AB75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="AC75" s="5" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+      <c r="AD75" s="6" t="str">
+        <f t="shared" si="30"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="76" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A76" s="4" t="str">
+        <f t="shared" ref="A76:AD76" si="31">IF(OR(A55=" ", A55=""),"-",A55)</f>
+        <v>-</v>
+      </c>
+      <c r="B76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="C76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="D76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="E76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="F76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="G76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="H76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="I76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="J76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="K76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="L76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="M76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="N76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="O76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="P76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="Q76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="R76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="S76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="T76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="U76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="V76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="W76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="X76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="Y76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="Z76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="AA76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="AB76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="AC76" s="5" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+      <c r="AD76" s="6" t="str">
+        <f t="shared" si="31"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="77" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A77" s="4" t="str">
+        <f t="shared" ref="A77:AD77" si="32">IF(OR(A56=" ", A56=""),"-",A56)</f>
+        <v>-</v>
+      </c>
+      <c r="B77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="C77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="D77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="E77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="F77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="G77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="H77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="I77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="J77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="K77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="L77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="M77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="N77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="O77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="P77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="Q77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="R77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="S77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="T77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="U77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="V77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="W77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="X77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="Y77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="Z77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="AA77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="AB77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="AC77" s="5" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+      <c r="AD77" s="6" t="str">
+        <f t="shared" si="32"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A78" s="4" t="str">
+        <f t="shared" ref="A78:AD78" si="33">IF(OR(A57=" ", A57=""),"-",A57)</f>
+        <v>-</v>
+      </c>
+      <c r="B78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="C78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="D78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="E78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="F78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="G78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="H78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="I78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="J78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="K78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="L78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="M78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="N78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="O78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="P78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="Q78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="R78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="S78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="T78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="U78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="V78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="W78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="X78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="Y78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="Z78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="AA78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="AB78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="AC78" s="5" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+      <c r="AD78" s="6" t="str">
+        <f t="shared" si="33"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A79" s="4" t="str">
+        <f t="shared" ref="A79:AD79" si="34">IF(OR(A58=" ", A58=""),"-",A58)</f>
+        <v>-</v>
+      </c>
+      <c r="B79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="C79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="D79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="E79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="F79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="G79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="H79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="I79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="J79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="K79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="L79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="M79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="N79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="O79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="P79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="Q79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="R79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="S79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="T79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="U79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="V79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="W79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="X79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="Y79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="Z79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="AA79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="AB79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="AC79" s="5" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+      <c r="AD79" s="6" t="str">
+        <f t="shared" si="34"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A80" s="4" t="str">
+        <f t="shared" ref="A80:AD80" si="35">IF(OR(A59=" ", A59=""),"-",A59)</f>
+        <v>-</v>
+      </c>
+      <c r="B80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="C80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="D80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="E80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="F80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="G80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="H80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="I80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="J80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="K80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="L80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="M80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="N80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="O80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="P80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="Q80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="R80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="S80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="T80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="U80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="V80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="W80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="X80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="Y80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="Z80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="AA80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="AB80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="AC80" s="5" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+      <c r="AD80" s="6" t="str">
+        <f t="shared" si="35"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A81" s="4" t="str">
+        <f t="shared" ref="A81:AD81" si="36">IF(OR(A60=" ", A60=""),"-",A60)</f>
+        <v>-</v>
+      </c>
+      <c r="B81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="C81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="D81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="E81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="F81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="G81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="H81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="I81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="J81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="K81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="L81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="M81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="N81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="O81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="P81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="Q81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="R81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="S81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="T81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="U81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="V81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="W81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="X81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="Y81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="Z81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="AA81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="AB81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="AC81" s="5" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+      <c r="AD81" s="6" t="str">
+        <f t="shared" si="36"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A82" s="4" t="str">
+        <f t="shared" ref="A82:AD82" si="37">IF(OR(A61=" ", A61=""),"-",A61)</f>
+        <v>-</v>
+      </c>
+      <c r="B82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="C82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="D82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="E82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="F82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="G82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="H82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="I82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="J82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="K82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="L82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="M82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="N82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="O82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="P82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="Q82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="R82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="S82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="T82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="U82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="V82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="W82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="X82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="Y82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="Z82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="AA82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="AB82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="AC82" s="5" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+      <c r="AD82" s="6" t="str">
+        <f t="shared" si="37"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A83" s="4" t="str">
+        <f t="shared" ref="A83:AD83" si="38">IF(OR(A62=" ", A62=""),"-",A62)</f>
+        <v>-</v>
+      </c>
+      <c r="B83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="C83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="D83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="E83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="F83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="G83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="H83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="I83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="J83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="K83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="L83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="M83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="N83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="O83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="P83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="Q83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="R83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="S83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="T83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="U83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="V83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="W83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="X83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="Y83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="Z83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="AA83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="AB83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="AC83" s="5" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+      <c r="AD83" s="6" t="str">
+        <f t="shared" si="38"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+      <c r="A84" s="4" t="str">
+        <f t="shared" ref="A84:AD84" si="39">IF(OR(A63=" ", A63=""),"-",A63)</f>
+        <v>-</v>
+      </c>
+      <c r="B84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="C84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="D84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="E84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="F84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="G84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="H84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="I84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="J84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="K84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="L84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="M84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="N84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="O84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="P84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="Q84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="R84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="S84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="T84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="U84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="V84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="W84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="X84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="Y84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="Z84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="AA84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="AB84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="AC84" s="5" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+      <c r="AD84" s="6" t="str">
+        <f t="shared" si="39"/>
+        <v>-</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A85" s="7" t="str">
+        <f t="shared" ref="A85:AD85" si="40">IF(OR(A64=" ", A64=""),"-",A64)</f>
+        <v>-</v>
+      </c>
+      <c r="B85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="C85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="D85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="E85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="F85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="G85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="H85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="I85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="J85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="K85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="L85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="M85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="N85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="O85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="P85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="Q85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="R85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="S85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="T85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="U85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="V85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="W85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="X85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="Y85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="Z85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="AA85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="AB85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="AC85" s="8" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+      <c r="AD85" s="9" t="str">
+        <f t="shared" si="40"/>
+        <v>-</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="AG24:AL24"/>

</xml_diff>